<commit_message>
sjs_yfg_pdm - bug fix
</commit_message>
<xml_diff>
--- a/src/main/resources/excelTemp/planningTempInit-test.xlsx
+++ b/src/main/resources/excelTemp/planningTempInit-test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="287">
   <si>
     <t>特殊需求</t>
   </si>
@@ -68,16 +68,16 @@
     <t>小类</t>
   </si>
   <si>
-    <t>目标销价</t>
-  </si>
-  <si>
-    <t>目标销价区间</t>
+    <t>目标销价终止</t>
   </si>
   <si>
     <t>企划目标倍率</t>
   </si>
   <si>
     <t>目标成本</t>
+  </si>
+  <si>
+    <t>款图</t>
   </si>
   <si>
     <t>家居</t>
@@ -2047,10 +2047,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58333333333333" defaultRowHeight="18.65" customHeight="1" outlineLevelRow="1"/>
@@ -2062,11 +2062,11 @@
     <col min="10" max="10" width="17.7833333333333" style="19" customWidth="1"/>
     <col min="11" max="11" width="15.375" style="20" customWidth="1"/>
     <col min="12" max="12" width="14.7166666666667" style="21" customWidth="1"/>
-    <col min="13" max="15" width="14.7166666666667" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="8.58333333333333" style="22"/>
+    <col min="13" max="16" width="14.7166666666667" style="19" customWidth="1"/>
+    <col min="17" max="16384" width="8.58333333333333" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="1" ht="14.25" spans="1:15">
+    <row r="1" s="15" customFormat="1" ht="14.25" spans="1:16">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2104,16 +2104,19 @@
         <v>11</v>
       </c>
       <c r="M1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="P1" s="25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" s="16" customFormat="1" ht="14.25" spans="1:15">
+    <row r="2" s="16" customFormat="1" ht="14.25" spans="1:16">
       <c r="A2" s="26"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -2129,10 +2132,11 @@
       <c r="M2" s="19"/>
       <c r="N2" s="19"/>
       <c r="O2" s="19"/>
+      <c r="P2" s="27"/>
     </row>
   </sheetData>
-  <dataValidations count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 B1 C1 D1 E$1:E$1048576 F$1:F$1048576 G$1:G$1048576 H$1:H$1048576"/>
+  <dataValidations count="10">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 B1 C1 D1 E$1:E$1048576 F$1:F$1048576 G$1:G$1048576 H$1:H$1048576 P$1:P$1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576 B2:B1048576">
       <formula1>"是,否"</formula1>
     </dataValidation>
@@ -2151,13 +2155,17 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576">
       <formula1>OFFSET(子产品线,,MATCH($J2,产品线,)-1,COUNTA(OFFSET(子产品线,,MATCH($J2,产品线,)-1,65535)))</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576 N$1:N$1048576 O$1:O$1048576">
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L$1:L$1048576">
       <formula1>0</formula1>
-      <formula2>1000000000</formula2>
+      <formula2>1000000</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M$1:M$1048576">
       <formula1>0</formula1>
       <formula2>10000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N$1:N$1048576 O$1:O$1048576">
+      <formula1>0</formula1>
+      <formula2>1000000000</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>